<commit_message>
adding feature of adding and deleting rows in periodicMaintenance page
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/maintenanceRequest.xlsx
+++ b/src/main/resources/templates/maintenanceRequest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,11 +188,11 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,8 +503,8 @@
   </sheetPr>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,11 +513,11 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" x14ac:dyDescent="0.35">
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
@@ -631,8 +631,8 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="27.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -888,7 +888,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="4"/>

</xml_diff>